<commit_message>
Added More Pages and TestCases
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naimatullah.khan_ven\Downloads\Automation\page-object-model\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521FCA1F-AE21-4B62-9537-6BC4AAACDF8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBDC40C3-1D6A-4521-A9E1-289E7C957593}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +37,24 @@
   </si>
   <si>
     <t>standard_user</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>company</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>hello@gmail.com</t>
+  </si>
+  <si>
+    <t>Network</t>
+  </si>
+  <si>
+    <t>Hello I am Hello User</t>
   </si>
 </sst>
 </file>
@@ -89,11 +107,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -375,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -387,27 +404,48 @@
     <col min="2" max="2" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{90545C3F-BC4D-4FF0-9512-0606E26BBC60}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>